<commit_message>
Fix Heatmap side pixels colorset
</commit_message>
<xml_diff>
--- a/ddSpaceGLONASSCoord.xlsx
+++ b/ddSpaceGLONASSCoord.xlsx
@@ -61,8 +61,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="3.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -70,7 +70,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="2">
@@ -78,7 +78,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.7320508075688528</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="3">
@@ -86,7 +86,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4.28024963002555</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="4">
@@ -94,7 +94,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>6.595676204819444</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="5">
@@ -102,7 +102,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>8.65888005625063</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="6">
@@ -110,7 +110,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>10.890494916554292</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="7">
@@ -118,7 +118,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>13.465308925672417</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="8">
@@ -126,7 +126,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>15.354591827301787</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="9">
@@ -134,7 +134,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>17.96766729997402</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="10">
@@ -142,7 +142,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>19.45359705479784</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="11">
@@ -150,7 +150,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>21.883527852030845</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="12">
@@ -158,7 +158,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>25.02882246566892</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="13">
@@ -166,7 +166,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>27.378277123111985</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="14">
@@ -174,7 +174,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>29.54138445705573</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="15">
@@ -182,7 +182,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>30.658345259235233</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="16">
@@ -190,7 +190,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>33.31884158255825</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="17">
@@ -198,7 +198,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>35.674753143660126</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="18">
@@ -206,7 +206,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>37.84831033518492</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="19">
@@ -214,7 +214,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>39.512589761896265</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="20">
@@ -222,7 +222,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>42.14946556979528</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="21">
@@ -230,7 +230,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>44.02978710970046</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="22">
@@ -238,7 +238,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>45.772201268422705</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="23">
@@ -246,7 +246,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>49.07116453270851</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="24">
@@ -254,7 +254,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>51.96072672803421</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="25">
@@ -262,7 +262,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>53.26875730796485</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="26">
@@ -270,7 +270,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>56.45344554954013</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="27">
@@ -278,7 +278,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>57.1365374216479</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="28">
@@ -286,7 +286,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>58.38212853103981</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="29">
@@ -294,7 +294,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>63.67129345195688</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="30">
@@ -302,7 +302,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>64.41518268201719</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="31">
@@ -310,7 +310,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>66.9339652552259</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="32">
@@ -318,7 +318,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>68.14196728441117</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="33">
@@ -326,7 +326,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>71.76815653542035</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="34">
@@ -334,7 +334,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>72.57046848473911</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="35">
@@ -342,7 +342,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>77.1834992013355</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="36">
@@ -350,7 +350,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>77.27642403255922</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="37">
@@ -358,7 +358,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>80.9027703767394</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="38">
@@ -366,7 +366,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>82.14848460040153</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="39">
@@ -374,7 +374,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>84.46070286663259</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="40">
@@ -382,7 +382,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>84.35359232088051</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="41">
@@ -390,7 +390,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>89.60762987844548</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="42">
@@ -398,7 +398,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>93.09665506572053</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="43">
@@ -406,7 +406,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>96.7352213921698</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="44">
@@ -414,7 +414,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>96.65129187188299</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="45">
@@ -422,7 +422,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>96.91157241140185</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="46">
@@ -430,7 +430,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>97.98362622099863</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="47">
@@ -438,7 +438,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>103.79776336851913</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="48">
@@ -446,7 +446,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>105.31277385819301</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="49">
@@ -454,7 +454,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>104.7812187669936</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="50">
@@ -462,7 +462,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>104.36328023403095</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="51">
@@ -470,7 +470,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>110.19448450418078</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="52">
@@ -478,7 +478,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>111.40130017323425</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="53">
@@ -486,7 +486,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>116.11919587436887</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="54">
@@ -494,7 +494,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>115.76902388702845</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="55">
@@ -502,7 +502,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>118.76603543037125</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="56">
@@ -510,7 +510,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>122.79891916637062</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="57">
@@ -518,7 +518,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>121.85827453076679</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="58">
@@ -526,7 +526,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>126.57249081218693</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="59">
@@ -534,7 +534,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>127.70856924602704</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="60">
@@ -542,7 +542,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>129.4382846789235</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="61">
@@ -550,7 +550,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>134.75883245788484</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="62">
@@ -558,7 +558,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>134.78121934212123</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="63">
@@ -566,7 +566,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>138.94855992296198</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="64">
@@ -574,7 +574,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>139.80632758467706</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="65">
@@ -582,7 +582,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>138.78230022869408</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="66">
@@ -590,7 +590,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>144.9815022326422</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="67">
@@ -598,7 +598,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>150.15451115342728</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="68">
@@ -606,7 +606,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>145.89900626783242</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="69">
@@ -614,7 +614,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>149.10515635122962</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="70">
@@ -622,7 +622,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>152.42410163993472</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="71">
@@ -630,7 +630,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>154.97601516593696</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="72">
@@ -638,7 +638,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>157.77099436283513</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="73">
@@ -646,7 +646,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>160.48837218051145</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="74">
@@ -654,7 +654,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>158.94580228732266</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="75">
@@ -662,7 +662,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>161.9260262645984</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="76">
@@ -670,7 +670,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>167.6175356966645</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="77">
@@ -678,7 +678,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>165.39376840102545</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="78">
@@ -686,7 +686,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>172.86033816954836</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="79">
@@ -694,7 +694,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>173.1244161598298</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="80">
@@ -702,7 +702,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>173.77277319463104</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="81">
@@ -710,7 +710,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>177.02700235566488</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="82">
@@ -718,7 +718,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>181.04186493593411</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="83">
@@ -726,7 +726,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>176.77341517257878</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="84">
@@ -734,7 +734,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>178.93302332163407</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="85">
@@ -742,7 +742,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>184.58161149765567</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="86">
@@ -750,7 +750,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>193.77427857450147</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="87">
@@ -758,7 +758,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>193.78055640636796</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="88">
@@ -766,7 +766,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>193.4816541719485</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="89">
@@ -774,7 +774,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>195.31555107457507</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="90">
@@ -782,7 +782,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>195.1450439826571</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="91">
@@ -790,7 +790,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>199.82807804212868</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="92">
@@ -798,7 +798,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>195.97536527214666</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="93">
@@ -806,7 +806,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>198.9988296602227</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="94">
@@ -814,7 +814,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>211.34916808281667</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="95">
@@ -822,7 +822,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>208.58342290437025</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="96">
@@ -830,7 +830,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>206.6176331779961</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="97">
@@ -838,7 +838,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>212.77192528507481</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="98">
@@ -846,7 +846,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>215.0841608637745</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="99">
@@ -854,7 +854,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>217.5028767885365</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
     <row r="100">
@@ -862,7 +862,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>220.1770426101452</v>
+        <v>8660.25403784423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>